<commit_message>
v1.1 Updated the Testcases According to the review
LH_TC_IDCONSTRAINTS_Create_031
</commit_message>
<xml_diff>
--- a/LH_TESTCASES/LH_TC_IDCONSTRAINTS.xlsx
+++ b/LH_TESTCASES/LH_TC_IDCONSTRAINTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095EA415-08C9-484E-A2BF-96F43159D0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A991D66-724E-4E47-A9F8-5B65ABFA29CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_TC_FEATURENAME" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>Preconditions</t>
   </si>
@@ -115,25 +115,10 @@
     <t>High</t>
   </si>
   <si>
-    <t>TC_IDCONSTRAINTS_001</t>
-  </si>
-  <si>
-    <t>1. Enter valid email.
-2. Enter valid username.
-3. Enter valid password.
-4. Click Register.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ensuring generated user IDs follow the required format UXXX.  </t>
   </si>
   <si>
-    <t>TC_IDCONSTRAINTS_002</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Checking that user IDs are generated sequentially.</t>
-  </si>
-  <si>
-    <t>TC_IDCONSTRAINTS_003</t>
   </si>
   <si>
     <t>1-Email: user3@domain.com
@@ -164,17 +149,6 @@
     <t>Medium</t>
   </si>
   <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>1- Enter valid email.
-2- Enter valid username.
-3- Enter valid password.
-4- Click Register.
-5- note the user ID
-6- Register another new user with a different valid email, username, and password and then note the user ID</t>
-  </si>
-  <si>
     <t>1- The second user ID is the next sequential ID after the first user ID (e.g., if the first user ID is U001, the second is U002).</t>
   </si>
   <si>
@@ -195,6 +169,44 @@
   </si>
   <si>
     <t>SRS-ID-002.3</t>
+  </si>
+  <si>
+    <t>1. The system is operational.
+2. The user registration form is accessible.</t>
+  </si>
+  <si>
+    <t>1- Navigate to the sign up page on the browser
+2- Enter valid email.
+3- Enter valid username.
+4- Enter valid password.
+5- Click Register.
+5- note the user ID
+7- Register another new user with a different valid email, username, and password and then note the user ID</t>
+  </si>
+  <si>
+    <t>1- Navigate to the sign up page on the browser
+2- Enter valid email.
+3- Enter valid username.
+4- Enter valid password.
+5- Click Register.</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>LH-TC-IDCONSTRAINTS_001</t>
+  </si>
+  <si>
+    <t>LH-TC-IDCONSTRAINTS_002</t>
+  </si>
+  <si>
+    <t>LH-TC-IDCONSTRAINTS_003</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>Updated the testcases According to the review points</t>
   </si>
 </sst>
 </file>
@@ -377,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -443,6 +455,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -770,14 +783,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.77734375" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5546875" style="10" customWidth="1"/>
     <col min="3" max="3" width="41.88671875" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.21875" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.21875" style="10" bestFit="1" customWidth="1"/>
@@ -805,7 +818,9 @@
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="16"/>
+      <c r="B2" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="C2" s="17"/>
       <c r="D2" s="18"/>
       <c r="I2" s="22"/>
@@ -814,7 +829,9 @@
       <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="16"/>
+      <c r="B3" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="C3" s="17"/>
       <c r="D3" s="18"/>
       <c r="I3" s="22"/>
@@ -871,83 +888,83 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="11" customFormat="1" ht="189" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" s="11" customFormat="1" ht="231" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I9" s="24"/>
       <c r="J9" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="84" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="126" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="231" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="189" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>29</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -974,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1008,18 +1025,27 @@
         <v>20</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D2" s="7">
         <f ca="1">TODAY()</f>
-        <v>45767</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+        <v>45768</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="63" x14ac:dyDescent="0.4">
+      <c r="A3" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="7">
+        <f ca="1">TODAY()</f>
+        <v>45768</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>

</xml_diff>